<commit_message>
weka text classifier sample added
</commit_message>
<xml_diff>
--- a/FactorsAffectingSensex.xlsx
+++ b/FactorsAffectingSensex.xlsx
@@ -3,15 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{011171BB-29DB-4DFD-A402-030E045D591B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{142806E5-B34C-4024-B920-7ACC756E48F1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="sensex data" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,18 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>gdp</t>
   </si>
   <si>
     <t>iip</t>
-  </si>
-  <si>
-    <t>class-sensex-change</t>
-  </si>
-  <si>
-    <t>bank-rate</t>
   </si>
   <si>
     <t>mnth_infla</t>
@@ -50,17 +46,50 @@
     <t>DEBT</t>
   </si>
   <si>
-    <t>FII Equity</t>
+    <t>CLOSE</t>
   </si>
   <si>
-    <t>FII Debt</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>bank_rate</t>
+  </si>
+  <si>
+    <t>FII_Equity</t>
+  </si>
+  <si>
+    <t>FII_Debt</t>
+  </si>
+  <si>
+    <t>class_sensex_change</t>
+  </si>
+  <si>
+    <t>class_sensex_change_binary</t>
+  </si>
+  <si>
+    <t>POSITIVE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +122,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,8 +142,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -134,13 +175,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFDCDCDC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -170,6 +220,9 @@
     </xf>
     <xf numFmtId="4" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -453,22 +506,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B2" sqref="B2:I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -477,22 +531,25 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -514,8 +571,14 @@
       <c r="G2">
         <v>-2601.0700000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>94.889999999999418</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43435</v>
       </c>
@@ -537,8 +600,15 @@
       <c r="G3">
         <v>5804.98</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>-328.36000000000058</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I38" si="0">IF(H2&gt;0,"POSITIVE",IF(H2&lt;0,"NEGATIVE","ZERO"))</f>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43405</v>
       </c>
@@ -560,8 +630,15 @@
       <c r="G4">
         <v>2262.77</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>1543.6700000000055</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43374</v>
       </c>
@@ -583,8 +660,15 @@
       <c r="G5">
         <v>-10019.219999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>-1832.1999999999971</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43344</v>
       </c>
@@ -606,8 +690,15 @@
       <c r="G6">
         <v>-10527.94</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>-2688.7700000000041</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43313</v>
       </c>
@@ -629,8 +720,15 @@
       <c r="G7">
         <v>2366.77</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>1001.1999999999971</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43282</v>
       </c>
@@ -652,8 +750,15 @@
       <c r="G8">
         <v>178.22</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>2061.3600000000006</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43252</v>
       </c>
@@ -675,8 +780,15 @@
       <c r="G9">
         <v>-10005.65</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>49.5</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43221</v>
       </c>
@@ -698,8 +810,15 @@
       <c r="G10">
         <v>-17543.09</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>-6.5300000000061118</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43191</v>
       </c>
@@ -721,8 +840,15 @@
       <c r="G11">
         <v>-11868.3</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>2129.489999999998</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43160</v>
       </c>
@@ -744,8 +870,15 @@
       <c r="G12">
         <v>-7297.82</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>-1172.5400000000009</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43132</v>
       </c>
@@ -767,8 +900,15 @@
       <c r="G13">
         <v>-2771.36</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>-1864.9499999999971</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43101</v>
       </c>
@@ -790,8 +930,15 @@
       <c r="G14">
         <v>8931.5499999999993</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>1905.0299999999988</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43070</v>
       </c>
@@ -813,8 +960,15 @@
       <c r="G15">
         <v>2463.2800000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>809.16999999999825</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43040</v>
       </c>
@@ -836,8 +990,15 @@
       <c r="G16">
         <v>-1426.4</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>-194.88000000000466</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43009</v>
       </c>
@@ -859,8 +1020,15 @@
       <c r="G17">
         <v>17960.72</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>1675.3199999999961</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42979</v>
       </c>
@@ -882,8 +1050,15 @@
       <c r="G18">
         <v>992.17</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>-485.61999999999898</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42948</v>
       </c>
@@ -905,8 +1080,15 @@
       <c r="G19">
         <v>15006.22</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>-849.30999999999767</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42917</v>
       </c>
@@ -928,8 +1110,15 @@
       <c r="G20">
         <v>17041.87</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>1358.8999999999978</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>42887</v>
       </c>
@@ -951,8 +1140,15 @@
       <c r="G21">
         <v>24796.34</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>-195.47999999999956</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42856</v>
       </c>
@@ -974,8 +1170,15 @@
       <c r="G22">
         <v>20197.919999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>1124.3099999999977</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>42826</v>
       </c>
@@ -997,8 +1200,15 @@
       <c r="G23">
         <v>19401.11</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>180.67000000000189</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42795</v>
       </c>
@@ -1020,8 +1230,15 @@
       <c r="G24">
         <v>26093.88</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>771.45999999999913</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>42767</v>
       </c>
@@ -1043,8 +1260,15 @@
       <c r="G25">
         <v>5980.19</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>1074.239999999998</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>42736</v>
       </c>
@@ -1066,8 +1290,15 @@
       <c r="G26">
         <v>-3757.43</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>944.80999999999767</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>42705</v>
       </c>
@@ -1089,8 +1320,15 @@
       <c r="G27">
         <v>-18902.53</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>-130.20000000000073</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>42675</v>
       </c>
@@ -1112,8 +1350,15 @@
       <c r="G28">
         <v>-19603.060000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>-1313.369999999999</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>42644</v>
       </c>
@@ -1135,8 +1380,15 @@
       <c r="G29">
         <v>-7151.88</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>-67.080000000001746</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>42614</v>
       </c>
@@ -1158,8 +1410,15 @@
       <c r="G30">
         <v>10577.04</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>-593.13000000000102</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>42583</v>
       </c>
@@ -1181,8 +1440,15 @@
       <c r="G31">
         <v>-2949.07</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>369.08999999999651</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>42552</v>
       </c>
@@ -1204,8 +1470,15 @@
       <c r="G32">
         <v>7382.28</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>987.52999999999884</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>42522</v>
       </c>
@@ -1227,8 +1500,15 @@
       <c r="G33">
         <v>-6505.58</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>315.26000000000204</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>42491</v>
       </c>
@@ -1250,8 +1530,15 @@
       <c r="G34">
         <v>-5171.38</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>1102.5200000000004</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>42461</v>
       </c>
@@ -1273,8 +1560,15 @@
       <c r="G35">
         <v>2948.39</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>304.91999999999825</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>42430</v>
       </c>
@@ -1296,8 +1590,15 @@
       <c r="G36">
         <v>4547.6400000000003</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>2188.5400000000009</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>42401</v>
       </c>
@@ -1319,8 +1620,15 @@
       <c r="G37">
         <v>-8324.2000000000007</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>-1980.2200000000012</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="0"/>
+        <v>POSITIVE</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>42370</v>
       </c>
@@ -1341,6 +1649,13 @@
       </c>
       <c r="G38">
         <v>10741</v>
+      </c>
+      <c r="H38">
+        <v>-1230.8100000000013</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="0"/>
+        <v>NEGATIVE</v>
       </c>
     </row>
   </sheetData>
@@ -1349,6 +1664,887 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18D041F-04F6-470F-A379-C724A2FC3BF1}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B2">
+        <v>36256.69</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43435</v>
+      </c>
+      <c r="B3">
+        <v>36068.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43405</v>
+      </c>
+      <c r="B4">
+        <v>36194.300000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43374</v>
+      </c>
+      <c r="B5">
+        <v>34442.050000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43344</v>
+      </c>
+      <c r="B6">
+        <v>36227.14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C9FE0D-F038-4184-BB85-F2AF755226A3}">
+  <dimension ref="A1:F38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B2">
+        <v>36161.800000000003</v>
+      </c>
+      <c r="C2">
+        <v>36701.03</v>
+      </c>
+      <c r="D2">
+        <v>35375.51</v>
+      </c>
+      <c r="E2">
+        <v>36256.69</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F38" si="0">E2-B2</f>
+        <v>94.889999999999418</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43435</v>
+      </c>
+      <c r="B3">
+        <v>36396.69</v>
+      </c>
+      <c r="C3">
+        <v>36554.99</v>
+      </c>
+      <c r="D3">
+        <v>34426.29</v>
+      </c>
+      <c r="E3">
+        <v>36068.33</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>-328.36000000000058</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43405</v>
+      </c>
+      <c r="B4">
+        <v>34650.629999999997</v>
+      </c>
+      <c r="C4">
+        <v>36389.22</v>
+      </c>
+      <c r="D4">
+        <v>34303.379999999997</v>
+      </c>
+      <c r="E4">
+        <v>36194.300000000003</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>1543.6700000000055</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43374</v>
+      </c>
+      <c r="B5">
+        <v>36274.25</v>
+      </c>
+      <c r="C5">
+        <v>36616.639999999999</v>
+      </c>
+      <c r="D5">
+        <v>33291.58</v>
+      </c>
+      <c r="E5">
+        <v>34442.050000000003</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>-1832.1999999999971</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43344</v>
+      </c>
+      <c r="B6">
+        <v>38915.910000000003</v>
+      </c>
+      <c r="C6">
+        <v>38934.35</v>
+      </c>
+      <c r="D6">
+        <v>35985.629999999997</v>
+      </c>
+      <c r="E6">
+        <v>36227.14</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>-2688.7700000000041</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43313</v>
+      </c>
+      <c r="B7">
+        <v>37643.870000000003</v>
+      </c>
+      <c r="C7">
+        <v>38989.65</v>
+      </c>
+      <c r="D7">
+        <v>37128.99</v>
+      </c>
+      <c r="E7">
+        <v>38645.07</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1001.1999999999971</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43282</v>
+      </c>
+      <c r="B8">
+        <v>35545.22</v>
+      </c>
+      <c r="C8">
+        <v>37644.589999999997</v>
+      </c>
+      <c r="D8">
+        <v>35106.57</v>
+      </c>
+      <c r="E8">
+        <v>37606.58</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>2061.3600000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43252</v>
+      </c>
+      <c r="B9">
+        <v>35373.980000000003</v>
+      </c>
+      <c r="C9">
+        <v>35877.410000000003</v>
+      </c>
+      <c r="D9">
+        <v>34784.68</v>
+      </c>
+      <c r="E9">
+        <v>35423.480000000003</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43221</v>
+      </c>
+      <c r="B10">
+        <v>35328.910000000003</v>
+      </c>
+      <c r="C10">
+        <v>35993.53</v>
+      </c>
+      <c r="D10">
+        <v>34302.89</v>
+      </c>
+      <c r="E10">
+        <v>35322.379999999997</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>-6.5300000000061118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43191</v>
+      </c>
+      <c r="B11">
+        <v>33030.870000000003</v>
+      </c>
+      <c r="C11">
+        <v>35213.300000000003</v>
+      </c>
+      <c r="D11">
+        <v>32972.559999999998</v>
+      </c>
+      <c r="E11">
+        <v>35160.36</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>2129.489999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43160</v>
+      </c>
+      <c r="B12">
+        <v>34141.22</v>
+      </c>
+      <c r="C12">
+        <v>34278.629999999997</v>
+      </c>
+      <c r="D12">
+        <v>32483.84</v>
+      </c>
+      <c r="E12">
+        <v>32968.68</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>-1172.5400000000009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43132</v>
+      </c>
+      <c r="B13">
+        <v>36048.99</v>
+      </c>
+      <c r="C13">
+        <v>36256.83</v>
+      </c>
+      <c r="D13">
+        <v>33482.81</v>
+      </c>
+      <c r="E13">
+        <v>34184.04</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>-1864.9499999999971</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43101</v>
+      </c>
+      <c r="B14">
+        <v>34059.99</v>
+      </c>
+      <c r="C14">
+        <v>36443.980000000003</v>
+      </c>
+      <c r="D14">
+        <v>33703.370000000003</v>
+      </c>
+      <c r="E14">
+        <v>35965.019999999997</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>1905.0299999999988</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43070</v>
+      </c>
+      <c r="B15">
+        <v>33247.660000000003</v>
+      </c>
+      <c r="C15">
+        <v>34137.97</v>
+      </c>
+      <c r="D15">
+        <v>32565.16</v>
+      </c>
+      <c r="E15">
+        <v>34056.83</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>809.16999999999825</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43040</v>
+      </c>
+      <c r="B16">
+        <v>33344.230000000003</v>
+      </c>
+      <c r="C16">
+        <v>33865.949999999997</v>
+      </c>
+      <c r="D16">
+        <v>32683.59</v>
+      </c>
+      <c r="E16">
+        <v>33149.35</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>-194.88000000000466</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43009</v>
+      </c>
+      <c r="B17">
+        <v>31537.81</v>
+      </c>
+      <c r="C17">
+        <v>33340.17</v>
+      </c>
+      <c r="D17">
+        <v>31440.48</v>
+      </c>
+      <c r="E17">
+        <v>33213.129999999997</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>1675.3199999999961</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>42979</v>
+      </c>
+      <c r="B18">
+        <v>31769.34</v>
+      </c>
+      <c r="C18">
+        <v>32524.11</v>
+      </c>
+      <c r="D18">
+        <v>31081.83</v>
+      </c>
+      <c r="E18">
+        <v>31283.72</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>-485.61999999999898</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>42948</v>
+      </c>
+      <c r="B19">
+        <v>32579.8</v>
+      </c>
+      <c r="C19">
+        <v>32686.48</v>
+      </c>
+      <c r="D19">
+        <v>31128.02</v>
+      </c>
+      <c r="E19">
+        <v>31730.49</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>-849.30999999999767</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>42917</v>
+      </c>
+      <c r="B20">
+        <v>31156.04</v>
+      </c>
+      <c r="C20">
+        <v>32672.66</v>
+      </c>
+      <c r="D20">
+        <v>31017.11</v>
+      </c>
+      <c r="E20">
+        <v>32514.94</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>1358.8999999999978</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>42887</v>
+      </c>
+      <c r="B21">
+        <v>31117.09</v>
+      </c>
+      <c r="C21">
+        <v>31522.87</v>
+      </c>
+      <c r="D21">
+        <v>30680.66</v>
+      </c>
+      <c r="E21">
+        <v>30921.61</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>-195.47999999999956</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>42856</v>
+      </c>
+      <c r="B22">
+        <v>30021.49</v>
+      </c>
+      <c r="C22">
+        <v>31255.279999999999</v>
+      </c>
+      <c r="D22">
+        <v>29804.12</v>
+      </c>
+      <c r="E22">
+        <v>31145.8</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>1124.3099999999977</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>42826</v>
+      </c>
+      <c r="B23">
+        <v>29737.73</v>
+      </c>
+      <c r="C23">
+        <v>30184.22</v>
+      </c>
+      <c r="D23">
+        <v>29241.48</v>
+      </c>
+      <c r="E23">
+        <v>29918.400000000001</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>180.67000000000189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>42795</v>
+      </c>
+      <c r="B24">
+        <v>28849.040000000001</v>
+      </c>
+      <c r="C24">
+        <v>29824.62</v>
+      </c>
+      <c r="D24">
+        <v>28716.21</v>
+      </c>
+      <c r="E24">
+        <v>29620.5</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>771.45999999999913</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>42767</v>
+      </c>
+      <c r="B25">
+        <v>27669.08</v>
+      </c>
+      <c r="C25">
+        <v>29065.31</v>
+      </c>
+      <c r="D25">
+        <v>27590.1</v>
+      </c>
+      <c r="E25">
+        <v>28743.32</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>1074.239999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>42736</v>
+      </c>
+      <c r="B26">
+        <v>26711.15</v>
+      </c>
+      <c r="C26">
+        <v>27980.39</v>
+      </c>
+      <c r="D26">
+        <v>26447.06</v>
+      </c>
+      <c r="E26">
+        <v>27655.96</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>944.80999999999767</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>42705</v>
+      </c>
+      <c r="B27">
+        <v>26756.66</v>
+      </c>
+      <c r="C27">
+        <v>26803.759999999998</v>
+      </c>
+      <c r="D27">
+        <v>25753.74</v>
+      </c>
+      <c r="E27">
+        <v>26626.46</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>-130.20000000000073</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>42675</v>
+      </c>
+      <c r="B28">
+        <v>27966.18</v>
+      </c>
+      <c r="C28">
+        <v>28029.8</v>
+      </c>
+      <c r="D28">
+        <v>25717.93</v>
+      </c>
+      <c r="E28">
+        <v>26652.81</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>-1313.369999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>42644</v>
+      </c>
+      <c r="B29">
+        <v>27997.29</v>
+      </c>
+      <c r="C29">
+        <v>28477.65</v>
+      </c>
+      <c r="D29">
+        <v>27488.3</v>
+      </c>
+      <c r="E29">
+        <v>27930.21</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>-67.080000000001746</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>42614</v>
+      </c>
+      <c r="B30">
+        <v>28459.09</v>
+      </c>
+      <c r="C30">
+        <v>29077.279999999999</v>
+      </c>
+      <c r="D30">
+        <v>27716.78</v>
+      </c>
+      <c r="E30">
+        <v>27865.96</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>-593.13000000000102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>42583</v>
+      </c>
+      <c r="B31">
+        <v>28083.08</v>
+      </c>
+      <c r="C31">
+        <v>28532.25</v>
+      </c>
+      <c r="D31">
+        <v>27627.97</v>
+      </c>
+      <c r="E31">
+        <v>28452.17</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>369.08999999999651</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>42552</v>
+      </c>
+      <c r="B32">
+        <v>27064.33</v>
+      </c>
+      <c r="C32">
+        <v>28240.2</v>
+      </c>
+      <c r="D32">
+        <v>27034.14</v>
+      </c>
+      <c r="E32">
+        <v>28051.86</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>987.52999999999884</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>42522</v>
+      </c>
+      <c r="B33">
+        <v>26684.46</v>
+      </c>
+      <c r="C33">
+        <v>27105.41</v>
+      </c>
+      <c r="D33">
+        <v>25911.33</v>
+      </c>
+      <c r="E33">
+        <v>26999.72</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>315.26000000000204</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>42491</v>
+      </c>
+      <c r="B34">
+        <v>25565.439999999999</v>
+      </c>
+      <c r="C34">
+        <v>26837.200000000001</v>
+      </c>
+      <c r="D34">
+        <v>25057.93</v>
+      </c>
+      <c r="E34">
+        <v>26667.96</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>1102.5200000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>42461</v>
+      </c>
+      <c r="B35">
+        <v>25301.7</v>
+      </c>
+      <c r="C35">
+        <v>26100.54</v>
+      </c>
+      <c r="D35">
+        <v>24523.200000000001</v>
+      </c>
+      <c r="E35">
+        <v>25606.62</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>304.91999999999825</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>42430</v>
+      </c>
+      <c r="B36">
+        <v>23153.32</v>
+      </c>
+      <c r="C36">
+        <v>25479.62</v>
+      </c>
+      <c r="D36">
+        <v>23133.18</v>
+      </c>
+      <c r="E36">
+        <v>25341.86</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>2188.5400000000009</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>42401</v>
+      </c>
+      <c r="B37">
+        <v>24982.22</v>
+      </c>
+      <c r="C37">
+        <v>25002.32</v>
+      </c>
+      <c r="D37">
+        <v>22494.61</v>
+      </c>
+      <c r="E37">
+        <v>23002</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>-1980.2200000000012</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>42370</v>
+      </c>
+      <c r="B38">
+        <v>26101.5</v>
+      </c>
+      <c r="C38">
+        <v>26197.27</v>
+      </c>
+      <c r="D38">
+        <v>23839.759999999998</v>
+      </c>
+      <c r="E38">
+        <v>24870.69</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>-1230.8100000000013</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8924AD57-0C1C-41DC-ACD0-0A4EC40D67F8}">
   <dimension ref="A1:C38"/>
   <sheetViews>
@@ -1365,15 +2561,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3">
         <v>-504.54</v>

</xml_diff>